<commit_message>
changed current 2020-Sem1-CAES-Wvl problem instance to <>-OLD and made a new 2020-Sem1-CAES-Wvl problem instance folder
- Due to discovering more CAES courses with their scheduled practical timetables in the CAES data given
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl/Students.xlsx
+++ b/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl/Students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\2020-Sem1-CAES-Wvl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDFCD36-8AAB-4BC4-8CCB-81CD353A69F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC33904A-7274-4BAF-9360-6A526BADA95B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="60" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10832,8 +10832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2548"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2025" workbookViewId="0">
-      <selection activeCell="C2030" sqref="C2030"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>